<commit_message>
added allocation by production volume
</commit_message>
<xml_diff>
--- a/dev/unlinked_exchanges.xlsx
+++ b/dev/unlinked_exchanges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akim/PycharmProjects/bigfood_db/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404C1044-9CBA-394D-9701-135875669821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9938F1C-F5FA-AE4F-B866-91A9ABDFC225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="460" windowWidth="33040" windowHeight="19700" xr2:uid="{E4C8F1BC-9FE2-C34F-96CF-F95EDBD4D09C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="176">
   <si>
     <t>Should be linked to</t>
   </si>
@@ -6271,9 +6271,6 @@
     <t>market for potassium chloride</t>
   </si>
   <si>
-    <t>no RER location, only RER w/o RU and RU</t>
-  </si>
-  <si>
     <t>TODO Claudio, can't find these in ecoinvent, maybe they should be added as new activities?</t>
   </si>
   <si>
@@ -6294,7 +6291,16 @@
     <t>search for "zinc scrap"</t>
   </si>
   <si>
-    <t>TODO Sasha</t>
+    <t>no RER location, only AT and Europe without Austria</t>
+  </si>
+  <si>
+    <t>no RER location, only CH and Europe without Switzerland</t>
+  </si>
+  <si>
+    <t>same as above but RER location</t>
+  </si>
+  <si>
+    <t>no RER location, only RER w/o RU and RU. Note that this one also has 2 reference products</t>
   </si>
 </sst>
 </file>
@@ -6344,7 +6350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6381,6 +6387,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6394,7 +6406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6435,9 +6447,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6446,6 +6455,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6769,8 +6787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952416DC-22EE-524A-BDFF-374D3425D5BC}">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6861,11 +6879,11 @@
       <c r="D6" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F6" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -6876,11 +6894,11 @@
       <c r="D7" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -6889,6 +6907,9 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
+      <c r="F8" s="5" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -7032,7 +7053,7 @@
         <v>105</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7044,7 +7065,7 @@
         <v>120</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>138</v>
       </c>
     </row>
@@ -7080,7 +7101,7 @@
         <v>119</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7092,7 +7113,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="17" t="s">
         <v>152</v>
       </c>
     </row>
@@ -7104,7 +7125,7 @@
         <v>96</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="14"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
@@ -7114,7 +7135,7 @@
         <v>109</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>153</v>
       </c>
     </row>
@@ -7126,7 +7147,7 @@
         <v>78</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -7134,11 +7155,11 @@
       <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
@@ -7170,31 +7191,31 @@
       <c r="A33" s="9">
         <v>31</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>33</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="16" t="s">
         <v>141</v>
       </c>
     </row>
@@ -7202,11 +7223,11 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
@@ -7316,51 +7337,51 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>44</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>45</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>46</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>47</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
@@ -7392,11 +7413,11 @@
       <c r="A52" s="9">
         <v>50</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
@@ -7406,7 +7427,7 @@
         <v>95</v>
       </c>
       <c r="C53" s="12"/>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>165</v>
       </c>
     </row>
@@ -7414,111 +7435,111 @@
       <c r="A54" s="9">
         <v>52</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>53</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>54</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>55</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>56</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>57</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>58</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>59</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>60</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>61</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>62</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
@@ -7536,11 +7557,11 @@
       <c r="A66" s="9">
         <v>64</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
@@ -7562,7 +7583,7 @@
         <v>97</v>
       </c>
       <c r="C68" s="12"/>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -7610,19 +7631,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
         <v>71</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>173</v>
-      </c>
+      <c r="C73" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D73" s="19"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
@@ -7681,7 +7700,7 @@
       <c r="B79" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="17" t="s">
         <v>144</v>
       </c>
       <c r="D79" s="12" t="s">
@@ -7695,7 +7714,7 @@
       <c r="B80" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C80" s="14"/>
+      <c r="C80" s="17"/>
       <c r="D80" s="12" t="s">
         <v>4</v>
       </c>
@@ -7708,7 +7727,7 @@
         <v>50</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>160</v>
@@ -7746,7 +7765,7 @@
         <v>121</v>
       </c>
       <c r="C84" s="12"/>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7754,25 +7773,25 @@
       <c r="A85" s="9">
         <v>83</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16" t="s">
-        <v>173</v>
-      </c>
+      <c r="C85" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D85" s="19"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>84</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16" t="s">
+      <c r="C86" s="19" t="s">
         <v>173</v>
       </c>
+      <c r="D86" s="19"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
@@ -7826,10 +7845,10 @@
         <v>66</v>
       </c>
       <c r="C91" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D91" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -7853,7 +7872,7 @@
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -7918,7 +7937,7 @@
         <v>102</v>
       </c>
       <c r="C99" s="12"/>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7980,7 +7999,7 @@
         <v>101</v>
       </c>
       <c r="C105" s="12"/>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -7992,7 +8011,7 @@
         <v>64</v>
       </c>
       <c r="C106" s="12"/>
-      <c r="D106" s="15" t="s">
+      <c r="D106" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -8016,7 +8035,7 @@
         <v>103</v>
       </c>
       <c r="C108" s="12"/>
-      <c r="D108" s="15" t="s">
+      <c r="D108" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -8028,7 +8047,7 @@
         <v>69</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>160</v>

</xml_diff>